<commit_message>
Updaed the Board Tags
</commit_message>
<xml_diff>
--- a/LAVA_Board_Tracker_Sheet.xlsx
+++ b/LAVA_Board_Tracker_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4E8404A-291B-445C-B555-9E85D4EEF4B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CE272D-1C73-4CC8-959D-1D512C70BB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4ED96E53-6AD2-4E18-9904-A92250FF6EF8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="147">
   <si>
     <t>Board241</t>
   </si>
@@ -475,9 +475,6 @@
   </si>
   <si>
     <t>Board-Type</t>
-  </si>
-  <si>
-    <t>A0 Raptor2</t>
   </si>
   <si>
     <t>TITAN</t>
@@ -548,9 +545,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -876,363 +876,363 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45FDD2B2-6FC9-4126-9EA0-C56A30B47DB2}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.26953125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.90625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.54296875" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.81640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="37" style="1" customWidth="1"/>
-    <col min="8" max="8" width="27.36328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="3.81640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="37" style="1" customWidth="1"/>
+    <col min="9" max="9" width="27.36328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="1">
         <v>241</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I3" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>102</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="C5" s="1">
         <v>114</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>74</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I5" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>119</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>75</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I6" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>120</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>76</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I7" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="C8" s="1">
         <v>121</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>77</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I8" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="C9" s="1">
         <v>122</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>78</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="C10" s="1">
         <v>123</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>79</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I10" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="C11" s="1">
         <v>124</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I11" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="C12" s="1">
         <v>125</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>81</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I12" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="C13" s="1">
         <v>126</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>82</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I13" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="C14" s="1">
         <v>130</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="E14" s="2" t="s">
         <v>83</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="C15" s="1">
         <v>131</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="E15" s="2" t="s">
         <v>84</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I15" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="C16" s="1">
         <v>133</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="E16" s="2" t="s">
         <v>85</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I16" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="C17" s="1">
         <v>134</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>86</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I17" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="C18" s="1">
         <v>135</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="E18" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G18" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1245,341 +1245,394 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819C40CE-D183-41A3-9DFA-7BB7CAA381A9}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.26953125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.90625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.6328125" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.81640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="37" style="1" customWidth="1"/>
-    <col min="8" max="8" width="27.36328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.26953125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.6328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="37" style="1" customWidth="1"/>
+    <col min="10" max="10" width="27.36328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="1">
         <v>136</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>88</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J3" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>229</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>89</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="C5" s="1">
         <v>203</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>90</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J5" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>204</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>91</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J6" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>211</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>92</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J7" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="C8" s="1">
         <v>219</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>93</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J8" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="C9" s="1">
         <v>220</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>94</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="C10" s="1">
         <v>221</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>95</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J10" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="C11" s="1">
         <v>222</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>96</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J11" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="C12" s="1">
         <v>223</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>97</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J12" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="C13" s="1">
         <v>225</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>98</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J13" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="C14" s="1">
         <v>226</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="E14" s="2" t="s">
         <v>99</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="C15" s="1">
         <v>244</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="E15" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J15" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="C16" s="1">
         <v>251</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="E16" s="2" t="s">
         <v>91</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J16" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="C17" s="1">
         <v>211</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1591,801 +1644,803 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5A988E-01F0-425F-A01C-25B2F7FD3DA1}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.26953125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.90625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.08984375" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.81640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="37" style="1" customWidth="1"/>
-    <col min="8" max="8" width="27.36328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="4.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="37" style="1" customWidth="1"/>
+    <col min="9" max="9" width="27.36328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>101</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I3" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>102</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I4" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="C5" s="1">
         <v>9</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>103</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I5" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>13</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>104</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I6" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>15</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>105</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I7" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="C8" s="1">
         <v>16</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>106</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I8" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="C9" s="1">
         <v>18</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>107</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I9" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="C10" s="1">
         <v>20</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>108</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I10" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="C11" s="1">
         <v>23</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>109</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I11" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="C12" s="1">
         <v>26</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>110</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I12" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="C13" s="1">
         <v>27</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>111</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I13" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="C14" s="1">
         <v>31</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="E14" s="2" t="s">
         <v>112</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I14" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="C15" s="1">
         <v>33</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="E15" s="2" t="s">
         <v>113</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I15" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="C16" s="1">
         <v>37</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="E16" s="2" t="s">
         <v>114</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I16" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="C17" s="1">
         <v>40</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>115</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I17" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="C18" s="1">
         <v>41</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="E18" s="2" t="s">
         <v>116</v>
       </c>
       <c r="G18" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I18" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="C19" s="1">
         <v>42</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F19" s="1" t="s">
+      <c r="E19" s="2" t="s">
         <v>117</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="C20" s="1">
         <v>43</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F20" s="1" t="s">
+      <c r="E20" s="2" t="s">
         <v>118</v>
       </c>
       <c r="G20" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I20" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="C21" s="1">
         <v>45</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F21" s="1" t="s">
+      <c r="E21" s="2" t="s">
         <v>119</v>
       </c>
       <c r="G21" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I21" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="C22" s="1">
         <v>46</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F22" s="1" t="s">
+      <c r="E22" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I22" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="C23" s="1">
         <v>47</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F23" s="1" t="s">
+      <c r="E23" s="2" t="s">
         <v>121</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I23" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="C24" s="1">
         <v>50</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F24" s="1" t="s">
+      <c r="E24" s="2" t="s">
         <v>122</v>
       </c>
       <c r="G24" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I24" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="C25" s="1">
         <v>51</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F25" s="1" t="s">
+      <c r="E25" s="2" t="s">
         <v>123</v>
       </c>
       <c r="G25" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I25" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="C26" s="1">
         <v>52</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F26" s="1" t="s">
+      <c r="E26" s="2" t="s">
         <v>124</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I26" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="C27" s="1">
         <v>56</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F27" s="1" t="s">
+      <c r="E27" s="2" t="s">
         <v>125</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I27" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="C28" s="1">
         <v>57</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F28" s="1" t="s">
+      <c r="E28" s="2" t="s">
         <v>126</v>
       </c>
       <c r="G28" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I28" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="C29" s="1">
         <v>59</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F29" s="1" t="s">
+      <c r="E29" s="2" t="s">
         <v>127</v>
       </c>
       <c r="G29" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I29" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="C30" s="1">
         <v>60</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F30" s="1" t="s">
+      <c r="E30" s="2" t="s">
         <v>128</v>
       </c>
       <c r="G30" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I30" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="C31" s="1">
         <v>61</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F31" s="1" t="s">
+      <c r="E31" s="2" t="s">
         <v>129</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I31" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="C32" s="1">
         <v>62</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F32" s="1" t="s">
+      <c r="E32" s="2" t="s">
         <v>130</v>
       </c>
       <c r="G32" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I32" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="C33" s="1">
         <v>63</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F33" s="1" t="s">
+      <c r="E33" s="2" t="s">
         <v>131</v>
       </c>
       <c r="G33" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I33" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="C34" s="1">
         <v>66</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F34" s="1" t="s">
+      <c r="E34" s="2" t="s">
         <v>132</v>
       </c>
       <c r="G34" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I34" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="C35" s="1">
         <v>67</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F35" s="1" t="s">
+      <c r="E35" s="2" t="s">
         <v>133</v>
       </c>
       <c r="G35" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I35" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="C36" s="1">
         <v>68</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F36" s="1" t="s">
+      <c r="E36" s="2" t="s">
         <v>134</v>
       </c>
       <c r="G36" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I36" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="C37" s="1">
         <v>69</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F37" s="1" t="s">
+      <c r="E37" s="2" t="s">
         <v>135</v>
       </c>
       <c r="G37" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I37" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="C38" s="1">
         <v>70</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F38" s="1" t="s">
+      <c r="E38" s="2" t="s">
         <v>136</v>
       </c>
       <c r="G38" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H38" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I38" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="C39" s="1">
         <v>72</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F39" s="1" t="s">
+      <c r="E39" s="2" t="s">
         <v>137</v>
       </c>
       <c r="G39" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I39" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="C40" s="1">
         <v>73</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F40" s="1" t="s">
+      <c r="E40" s="2" t="s">
         <v>138</v>
       </c>
       <c r="G40" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="I40" s="1" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>